<commit_message>
Created Graph by input data in excel
</commit_message>
<xml_diff>
--- a/HW3/DATA/data.xlsx
+++ b/HW3/DATA/data.xlsx
@@ -8,13 +8,46 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yiyanglin/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EDE7322-B501-D14F-A021-DAC8E32DAF7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F57B168-0656-A047-BA85-E14BE20D1CF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1680" yWindow="500" windowWidth="18800" windowHeight="12300" xr2:uid="{DC9075CF-ADB7-EE49-9E18-CBF0034BA20E}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20480" windowHeight="12800" xr2:uid="{DC9075CF-ADB7-EE49-9E18-CBF0034BA20E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId2"/>
+    <externalReference r:id="rId3"/>
+  </externalReferences>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">'[2]Core 64'!$A$11:$A$19</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">'[2]Core 64'!$B$11:$B$19</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">'[2]Core 64'!$B$11:$B$19</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">'[2]Core 64'!$B$9</definedName>
+    <definedName name="_xlchart.v1.12" hidden="1">'[2]Core 64'!$C$11:$C$19</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">'[2]Core 64'!$C$9</definedName>
+    <definedName name="_xlchart.v1.14" hidden="1">'[2]Core 64'!$D$11:$D$19</definedName>
+    <definedName name="_xlchart.v1.15" hidden="1">'[2]Core 64'!$D$9</definedName>
+    <definedName name="_xlchart.v1.16" hidden="1">'[2]Core 64'!$E$11:$E$19</definedName>
+    <definedName name="_xlchart.v1.17" hidden="1">'[2]Core 64'!$E$9</definedName>
+    <definedName name="_xlchart.v1.18" hidden="1">'[2]Core 64'!$A$11:$A$19</definedName>
+    <definedName name="_xlchart.v1.19" hidden="1">'[2]Core 64'!$B$11:$B$19</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">'[2]Core 64'!$B$9</definedName>
+    <definedName name="_xlchart.v1.20" hidden="1">'[2]Core 64'!$B$9</definedName>
+    <definedName name="_xlchart.v1.21" hidden="1">'[2]Core 64'!$C$11:$C$19</definedName>
+    <definedName name="_xlchart.v1.22" hidden="1">'[2]Core 64'!$C$9</definedName>
+    <definedName name="_xlchart.v1.23" hidden="1">'[2]Core 64'!$D$11:$D$19</definedName>
+    <definedName name="_xlchart.v1.24" hidden="1">'[2]Core 64'!$D$9</definedName>
+    <definedName name="_xlchart.v1.25" hidden="1">'[2]Core 64'!$E$11:$E$19</definedName>
+    <definedName name="_xlchart.v1.26" hidden="1">'[2]Core 64'!$E$9</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">'[2]Core 64'!$C$11:$C$19</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">'[2]Core 64'!$C$9</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">'[2]Core 64'!$D$11:$D$19</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">'[2]Core 64'!$D$9</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">'[2]Core 64'!$E$11:$E$19</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">'[2]Core 64'!$E$9</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">'[2]Core 64'!$A$11:$A$19</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -117,6 +150,37 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                    <a:prstClr val="black">
+                      <a:alpha val="40000"/>
+                    </a:prstClr>
+                  </a:outerShdw>
+                </a:effectLst>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Keyword: Conversational Agent</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -130,13 +194,19 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
                 </a:schemeClr>
               </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
@@ -149,29 +219,668 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
-        <c:grouping val="stacked"/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Lucene</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="9525" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="b"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="95000"/>
+                          <a:alpha val="54000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$1:$T$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>185</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>380</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>415</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>475</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>540</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>570</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>620</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>680</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>740</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$T$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>0.71399999999999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.86</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.5529999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.2149999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.47699999999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.79700000000000004</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.71</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>25.648</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.774</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.72</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>25.763000000000002</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.02</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>26.699000000000002</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.232</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>30.408999999999999</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.4219999999999999</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>26.013999999999999</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>32.738</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4.577</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000011-B8DE-D849-B2A6-AA422D00E4D9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>BF</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="9525" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent2">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent2">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="b"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="95000"/>
+                          <a:alpha val="54000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$1:$T$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>185</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>380</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>415</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>475</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>540</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>570</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>620</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>680</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>740</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$3:$T$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>1.1200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.9670000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.2570000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.83</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.5019999999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.2770000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.0549999999999997</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.3869999999999996</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.8390000000000004</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11.275</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>14.473000000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>16.173999999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>15.365</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>16.896000000000001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>18.994</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>19.655000000000001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>22.087</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>27.969000000000001</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>30.433</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000013-B8DE-D849-B2A6-AA422D00E4D9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
         <c:dLbls>
+          <c:dLblPos val="b"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="507161104"/>
-        <c:axId val="507176464"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="507161104"/>
+        <c:axId val="2127412544"/>
+        <c:axId val="2128303712"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2127412544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number of Articles</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="zh-TW"/>
+                  <a:t> </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>-</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="zh-TW"/>
+                  <a:t> </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>File</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="zh-TW"/>
+                  <a:t> </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Size </a:t>
+                </a:r>
+              </a:p>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="zh-TW"/>
+                  <a:t> </a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -179,12 +888,10 @@
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="50000"/>
               </a:schemeClr>
             </a:solidFill>
-            <a:round/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -195,9 +902,8 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -208,15 +914,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="507176464"/>
+        <c:crossAx val="2128303712"/>
         <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
       <c:valAx>
-        <c:axId val="507176464"/>
+        <c:axId val="2128303712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -226,9 +929,9 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -236,13 +939,71 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Respose Time (seconds)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln>
-            <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -253,9 +1014,8 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -266,9 +1026,9 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="507161104"/>
+        <c:crossAx val="2127412544"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -278,29 +1038,1046 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="zero"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
+    <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
+    <c:extLst/>
   </c:chart>
   <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                    <a:prstClr val="black">
+                      <a:alpha val="40000"/>
+                    </a:prstClr>
+                  </a:outerShdw>
+                </a:effectLst>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Keyword: Chatbot</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Lucene</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="9525" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="b"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="95000"/>
+                          <a:alpha val="54000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$6:$T$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>185</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>380</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>415</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>475</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>540</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>570</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>620</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>680</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>740</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$7:$T$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>0.44500000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.90300000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.4640000000000004</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.07</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.55</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>28.917999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.54700000000000004</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.54700000000000004</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.41</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>28.05</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.1240000000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.497</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>29.196000000000002</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>181.91</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>39.109000000000002</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>19.148</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>33.802</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>15.920999999999999</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>31.192</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8988-2C49-80CB-37986B15F151}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>BF</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="9525" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent2">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent2">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="b"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="95000"/>
+                          <a:alpha val="54000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$6:$T$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>185</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>380</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>415</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>475</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>540</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>570</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>620</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>680</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>740</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$8:$T$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>1.044</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.6259999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.2930000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0490000000000004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.9009999999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.891</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.3650000000000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.2799999999999994</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.0069999999999997</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9.8539999999999992</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>17.765999999999998</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>17.765999999999998</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13.35</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>15.744</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>21.847999999999999</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>20.6</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>25.295999999999999</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>23.332000000000001</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>25.273</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-8988-2C49-80CB-37986B15F151}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="b"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2127412544"/>
+        <c:axId val="2128303712"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2127412544"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number of Articles</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="zh-TW"/>
+                  <a:t> </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>-</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="zh-TW"/>
+                  <a:t> </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>File</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="zh-TW"/>
+                  <a:t> </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Size </a:t>
+                </a:r>
+              </a:p>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="zh-TW"/>
+                  <a:t> </a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2128303712"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2128303712"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Respose Time (seconds)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2127412544"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
     </a:ln>
     <a:effectLst/>
   </c:spPr>
@@ -362,63 +2139,107 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="248">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
     </cs:spPr>
     <cs:defRPr sz="1000" kern="1200"/>
   </cs:chartArea>
@@ -427,9 +2248,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
+      <a:schemeClr val="lt1">
         <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -448,14 +2268,6 @@
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
     <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
@@ -464,20 +2276,20 @@
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
@@ -486,13 +2298,13 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="28575" cap="rnd">
+      <a:ln w="9525" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -504,28 +2316,29 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
@@ -543,21 +2356,18 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -567,20 +2377,20 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -594,14 +2404,14 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
+        <a:prstDash val="dash"/>
       </a:ln>
     </cs:spPr>
   </cs:dropLine>
@@ -615,9 +2425,8 @@
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -631,12 +2440,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
   </cs:floor>
   <cs:gridlineMajor>
     <cs:lnRef idx="0"/>
@@ -648,9 +2451,9 @@
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -665,14 +2468,13 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln>
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:gridlineMinor>
@@ -684,14 +2486,14 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
+        <a:prstDash val="dash"/>
       </a:ln>
     </cs:spPr>
   </cs:hiLoLine>
@@ -703,14 +2505,13 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:leaderLine>
@@ -719,14 +2520,13 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+  <cs:plotArea>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
@@ -734,7 +2534,7 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+  <cs:plotArea3D>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
@@ -747,11 +2547,19 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:seriesAxis>
   <cs:seriesLine>
@@ -759,14 +2567,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -778,12 +2586,19 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -799,7 +2614,7 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:prstDash val="sysDot"/>
+        <a:prstDash val="sysDash"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -808,9 +2623,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -820,7 +2634,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -828,9 +2642,9 @@
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -841,11 +2655,521 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="248">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -855,12 +3179,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -869,23 +3187,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>260350</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>175683</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>477958</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>81936</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>704850</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>74083</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>169335</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
+        <xdr:cNvPr id="6" name="Chart 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{549BC013-4C2A-5703-8F8E-D1057368EE32}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BE09CF79-15FE-2647-4B01-47402469250C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -903,7 +3221,241 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>423333</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>176389</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>122676</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>138426</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Chart 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6CA323BD-E256-F54F-90DD-37A36AF370A6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Core 64"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Main"/>
+      <sheetName val="Core 64"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1">
+        <row r="9">
+          <cell r="B9" t="str">
+            <v>Passed</v>
+          </cell>
+          <cell r="C9" t="str">
+            <v>Failed</v>
+          </cell>
+          <cell r="D9" t="str">
+            <v>Errored</v>
+          </cell>
+          <cell r="E9" t="str">
+            <v>Blocked</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="A11" t="str">
+            <v>GFP4x4_PHY_IQexlm</v>
+          </cell>
+          <cell r="B11">
+            <v>6016</v>
+          </cell>
+          <cell r="C11">
+            <v>0</v>
+          </cell>
+          <cell r="D11">
+            <v>2</v>
+          </cell>
+          <cell r="E11">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="A12" t="str">
+            <v>TYP2x2_PHY_IQexlm</v>
+          </cell>
+          <cell r="B12">
+            <v>6035</v>
+          </cell>
+          <cell r="C12">
+            <v>5</v>
+          </cell>
+          <cell r="D12">
+            <v>0</v>
+          </cell>
+          <cell r="E12">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="A13" t="str">
+            <v>GFP2x2_PHY_IQexlm</v>
+          </cell>
+          <cell r="B13">
+            <v>5380</v>
+          </cell>
+          <cell r="C13">
+            <v>4</v>
+          </cell>
+          <cell r="D13">
+            <v>0</v>
+          </cell>
+          <cell r="E13">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="A14" t="str">
+            <v>HRP1x1_ANT_DIV_IQexlm</v>
+          </cell>
+          <cell r="B14">
+            <v>0</v>
+          </cell>
+          <cell r="C14">
+            <v>0</v>
+          </cell>
+          <cell r="D14">
+            <v>0</v>
+          </cell>
+          <cell r="E14">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="A15" t="str">
+            <v>HRP2x2_EXM</v>
+          </cell>
+          <cell r="B15">
+            <v>0</v>
+          </cell>
+          <cell r="C15">
+            <v>0</v>
+          </cell>
+          <cell r="D15">
+            <v>0</v>
+          </cell>
+          <cell r="E15">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="A16" t="str">
+            <v>QNJ+CCP2x2_EXM</v>
+          </cell>
+          <cell r="B16">
+            <v>1362</v>
+          </cell>
+          <cell r="C16">
+            <v>3</v>
+          </cell>
+          <cell r="D16">
+            <v>0</v>
+          </cell>
+          <cell r="E16">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="A17" t="str">
+            <v>SNJ+JFP1x1_EXM</v>
+          </cell>
+          <cell r="B17">
+            <v>946</v>
+          </cell>
+          <cell r="C17">
+            <v>0</v>
+          </cell>
+          <cell r="D17">
+            <v>0</v>
+          </cell>
+          <cell r="E17">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="A18" t="str">
+            <v>QNJ+JFP2x2_EXM</v>
+          </cell>
+          <cell r="B18">
+            <v>1218</v>
+          </cell>
+          <cell r="C18">
+            <v>21</v>
+          </cell>
+          <cell r="D18">
+            <v>0</v>
+          </cell>
+          <cell r="E18">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="A19" t="str">
+            <v>QNJ+JFP1x1_ANT_DIV_EXM</v>
+          </cell>
+          <cell r="B19">
+            <v>1162</v>
+          </cell>
+          <cell r="C19">
+            <v>12</v>
+          </cell>
+          <cell r="D19">
+            <v>0</v>
+          </cell>
+          <cell r="E19">
+            <v>0</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1205,8 +3757,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99909CC4-D88C-1147-9AED-D19DA0E6A757}">
   <dimension ref="A1:T8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="112" workbookViewId="0">
-      <selection activeCell="P11" sqref="P11"/>
+    <sheetView tabSelected="1" zoomScale="44" zoomScaleNormal="82" workbookViewId="0">
+      <selection activeCell="S25" sqref="S25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>